<commit_message>
checkpoint before add spreadsheet
</commit_message>
<xml_diff>
--- a/public/format/format-tahun-ajaran.xlsx
+++ b/public/format/format-tahun-ajaran.xlsx
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t xml:space="preserve">tahun ajaran</t>
-  </si>
-  <si>
-    <t xml:space="preserve">biaya</t>
   </si>
   <si>
     <t xml:space="preserve">keterangan</t>
@@ -131,37 +128,37 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="280" zoomScaleNormal="280" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="22.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="5.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="8" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="22.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="63" min="7" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1023" min="64" style="0" width="9.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1024" style="0" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -171,33 +168,21 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1250000</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="0" t="n">
-        <v>1500000</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>1750000</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>